<commit_message>
Add tests for adding payments to combined invoices
</commit_message>
<xml_diff>
--- a/tests/small_payments.xlsx
+++ b/tests/small_payments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grant/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grant/Sites/invoicing/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94B93A11-43DE-244F-8B10-734173E75FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C949E815-D92F-9347-84DE-397B3B2E1519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19320" yWindow="15100" windowWidth="38360" windowHeight="17620" xr2:uid="{B70FC92C-0E12-0A44-B98C-DE727DA052A9}"/>
   </bookViews>
@@ -96,10 +96,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$¥-804]#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,7 +452,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,6 +566,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>